<commit_message>
some changes in python code
</commit_message>
<xml_diff>
--- a/voting_right.xlsx
+++ b/voting_right.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F64284-4B5A-4DB8-A8F2-6BD0DED5D0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,11 +342,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -360,18 +361,602 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>314</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.73950000000000005</v>
+        <v>0.52310000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>574</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>0.74580000000000002</v>
+        <v>0.67730000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>0.53249999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>0.50270000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>112</v>
+      </c>
+      <c r="B8">
+        <v>0.60519999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>118</v>
+      </c>
+      <c r="B9">
+        <v>0.74219999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>0.71930000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>138</v>
+      </c>
+      <c r="B11">
+        <v>0.75980000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>155</v>
+      </c>
+      <c r="B12">
+        <v>0.3473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>159</v>
+      </c>
+      <c r="B13">
+        <v>0.51480000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>164</v>
+      </c>
+      <c r="B14">
+        <v>0.41889999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>165</v>
+      </c>
+      <c r="B15">
+        <v>0.61739999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>178</v>
+      </c>
+      <c r="B16">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>242</v>
+      </c>
+      <c r="B17">
+        <v>0.5474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>254</v>
+      </c>
+      <c r="B18">
+        <v>0.65959999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>321</v>
+      </c>
+      <c r="B19">
+        <v>0.83360000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>353</v>
+      </c>
+      <c r="B20">
+        <v>0.43790000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>355</v>
+      </c>
+      <c r="B21">
+        <v>0.34520000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>362</v>
+      </c>
+      <c r="B22">
+        <v>0.74590000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>373</v>
+      </c>
+      <c r="B23">
+        <v>0.432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>436</v>
+      </c>
+      <c r="B24">
+        <v>0.64249999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>448</v>
+      </c>
+      <c r="B25">
+        <v>0.3256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>452</v>
+      </c>
+      <c r="B26">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>459</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>486</v>
+      </c>
+      <c r="B28">
+        <v>0.75060000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>493</v>
+      </c>
+      <c r="B29">
+        <v>0.67390000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>494</v>
+      </c>
+      <c r="B30">
+        <v>0.50380000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>496</v>
+      </c>
+      <c r="B31">
+        <v>0.30759999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>535</v>
+      </c>
+      <c r="B32">
+        <v>0.52949999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>539</v>
+      </c>
+      <c r="B33">
+        <v>0.79010000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>548</v>
+      </c>
+      <c r="B34">
+        <v>0.64339999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>571</v>
+      </c>
+      <c r="B35">
+        <v>0.51139999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>573</v>
+      </c>
+      <c r="B36">
+        <v>0.58879999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>602</v>
+      </c>
+      <c r="B37">
+        <v>0.25269999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>604</v>
+      </c>
+      <c r="B38">
+        <v>0.51280000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>609</v>
+      </c>
+      <c r="B39">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>632</v>
+      </c>
+      <c r="B40">
+        <v>0.71279999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>652</v>
+      </c>
+      <c r="B41">
+        <v>0.82930000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>663</v>
+      </c>
+      <c r="B42">
+        <v>0.51439999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>669</v>
+      </c>
+      <c r="B43">
+        <v>0.65169999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>674</v>
+      </c>
+      <c r="B44">
+        <v>0.85819999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>676</v>
+      </c>
+      <c r="B45">
+        <v>0.58260000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>708</v>
+      </c>
+      <c r="B46">
+        <v>0.78149999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>719</v>
+      </c>
+      <c r="B47">
+        <v>0.57179999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>726</v>
+      </c>
+      <c r="B48">
+        <v>0.25629999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>751</v>
+      </c>
+      <c r="B49">
+        <v>0.3417</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>0.73029999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>126</v>
+      </c>
+      <c r="B51">
+        <v>0.42559999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>130</v>
+      </c>
+      <c r="B52">
+        <v>0.83689999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>133</v>
+      </c>
+      <c r="B53">
+        <v>0.83089999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>139</v>
+      </c>
+      <c r="B54">
+        <v>0.65810000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>151</v>
+      </c>
+      <c r="B55">
+        <v>0.63949999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>153</v>
+      </c>
+      <c r="B56">
+        <v>0.87529999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>154</v>
+      </c>
+      <c r="B57">
+        <v>0.89139999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>157</v>
+      </c>
+      <c r="B58">
+        <v>0.54310000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>186</v>
+      </c>
+      <c r="B59">
+        <v>0.48020000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>213</v>
+      </c>
+      <c r="B60">
+        <v>0.43469999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>330</v>
+      </c>
+      <c r="B61">
+        <v>0.50170000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>584</v>
+      </c>
+      <c r="B62">
+        <v>0.67710000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>585</v>
+      </c>
+      <c r="B63">
+        <v>0.50960000000000005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>591</v>
+      </c>
+      <c r="B64">
+        <v>0.33829999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>605</v>
+      </c>
+      <c r="B65">
+        <v>0.82220000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>606</v>
+      </c>
+      <c r="B66">
+        <v>0.85440000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>607</v>
+      </c>
+      <c r="B67">
+        <v>0.53280000000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>611</v>
+      </c>
+      <c r="B68">
+        <v>0.50860000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>636</v>
+      </c>
+      <c r="B69">
+        <v>0.54110000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>639</v>
+      </c>
+      <c r="B70">
+        <v>0.42699999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>668</v>
+      </c>
+      <c r="B71">
+        <v>0.56269999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>697</v>
+      </c>
+      <c r="B72">
+        <v>0.43819999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>752</v>
+      </c>
+      <c r="B73">
+        <v>0.47049999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>255</v>
+      </c>
+      <c r="B74">
+        <v>0.59519999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>278</v>
+      </c>
+      <c r="B75">
+        <v>0.66690000000000005</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>621</v>
+      </c>
+      <c r="B76">
+        <v>0.60660000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete data source for banks
</commit_message>
<xml_diff>
--- a/voting_right.xlsx
+++ b/voting_right.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C1160-548F-42B7-808A-6EDF40F58617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEC1B53-8584-4543-B162-9DF767C84087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,13 +343,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -361,106 +365,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>847</v>
       </c>
       <c r="B2">
-        <v>0.67730000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>16</v>
+        <v>848</v>
       </c>
       <c r="B3">
-        <v>0.76900000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>50</v>
+        <v>849</v>
       </c>
       <c r="B4">
-        <v>0.76200000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>112</v>
+        <v>850</v>
       </c>
       <c r="B5">
-        <v>0.60519999999999996</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>254</v>
+        <v>851</v>
       </c>
       <c r="B6">
-        <v>0.65959999999999996</v>
+        <v>0.98650000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>321</v>
+        <v>852</v>
       </c>
       <c r="B7">
-        <v>0.83360000000000001</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>355</v>
+        <v>853</v>
       </c>
       <c r="B8">
-        <v>0.34520000000000001</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>373</v>
+        <v>854</v>
       </c>
       <c r="B9">
-        <v>0.432</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>436</v>
+        <v>855</v>
       </c>
       <c r="B10">
-        <v>0.64249999999999996</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>535</v>
+        <v>856</v>
       </c>
       <c r="B11">
-        <v>0.52949999999999997</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>573</v>
+        <v>857</v>
       </c>
       <c r="B12">
-        <v>0.25140000000000001</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>719</v>
+        <v>858</v>
       </c>
       <c r="B13">
-        <v>0.57179999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>726</v>
-      </c>
-      <c r="B14">
-        <v>0.25629999999999997</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>